<commit_message>
Updated concrete recipe and added intro presentation
</commit_message>
<xml_diff>
--- a/materials/01_Concrete/101024_Concrete_mixdesign_mini_Eggshell_.xlsx
+++ b/materials/01_Concrete/101024_Concrete_mixdesign_mini_Eggshell_.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="126">
   <si>
     <t>Mixture:</t>
   </si>
@@ -433,54 +433,12 @@
     <t>Content</t>
   </si>
   <si>
-    <t>Composition pure components</t>
-  </si>
-  <si>
     <t>weight_solution_adm/weight_dry_binder</t>
   </si>
   <si>
     <t>Mass of accelerator C-100</t>
   </si>
   <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pen mes: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time </t>
-  </si>
-  <si>
-    <t xml:space="preserve">nr. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time of water add: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spread flow before acc: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time of acc: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time of place in pen container: </t>
-  </si>
-  <si>
-    <t>Time of entering the funnel</t>
-  </si>
-  <si>
-    <t>Time of starting filling of form:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time of starting deformation and friction measurement: </t>
-  </si>
-  <si>
-    <t>Force N</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Accelerator amount</t>
   </si>
   <si>
@@ -515,6 +473,12 @@
   </si>
   <si>
     <t>ACCELERATOR</t>
+  </si>
+  <si>
+    <t>ACCELERATION TABLE</t>
+  </si>
+  <si>
+    <t>&lt;--- edit this field</t>
   </si>
 </sst>
 </file>
@@ -677,18 +641,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -777,6 +741,303 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -892,7 +1153,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -916,16 +1177,10 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="11" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="11" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="97" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="3" borderId="3" xfId="12" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="11" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="11" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -933,10 +1188,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="12" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="12" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="12" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="22" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="22" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="23" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="24" xfId="12" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="12" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="29" xfId="12" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="31" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="30" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="31" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="12" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="10" xfId="12" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="15" xfId="11" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="12" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="112">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
@@ -2127,7 +2428,7 @@
       <c r="U23" t="s">
         <v>88</v>
       </c>
-      <c r="V23" s="25">
+      <c r="V23" s="24">
         <f>I20*(V32)</f>
         <v>0.43478260869565216</v>
       </c>
@@ -2179,7 +2480,7 @@
       <c r="H24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="25">
         <f>B28</f>
         <v>0.35</v>
       </c>
@@ -2387,7 +2688,7 @@
         <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>62</v>
@@ -2458,7 +2759,7 @@
         <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H28" s="18" t="s">
         <v>45</v>
@@ -2475,7 +2776,7 @@
       <c r="L28" t="s">
         <v>96</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="23"/>
       <c r="O28" s="6"/>
       <c r="AK28" s="14"/>
     </row>
@@ -2491,7 +2792,7 @@
         <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H29" s="18" t="s">
         <v>48</v>
@@ -2539,7 +2840,7 @@
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>51</v>
@@ -3584,10 +3885,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3603,126 +3904,112 @@
     <col min="13" max="13" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C1" t="str">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="79" t="str">
         <f>'M6'!B70</f>
         <v>Composition</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="39">
+      <c r="B2" s="43"/>
+      <c r="C2" s="74">
         <v>10000</v>
       </c>
       <c r="D2" t="str">
         <f>'M6'!C71</f>
         <v>mL</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="31"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C3" s="17"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="31"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="31"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" t="str">
+      <c r="E2" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="34"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="47"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="52"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="27"/>
+    </row>
+    <row r="5" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="34" t="str">
         <f>'M6'!A72</f>
         <v>Sand</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="35">
         <v>52</v>
       </c>
       <c r="D5" t="str">
         <f>'M6'!C72</f>
         <v>%</v>
       </c>
-      <c r="E5" t="str">
-        <f>'M6'!D72</f>
-        <v>Volume parts, all</v>
-      </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="31"/>
-    </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="36"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="31"/>
-    </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="36"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="31"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="64"/>
+    </row>
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="37"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="34"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="37"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="26"/>
+    </row>
+    <row r="8" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="B8" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="35">
         <f>100-C9-C10</f>
         <v>92</v>
       </c>
@@ -3730,147 +4017,193 @@
         <f>'M6'!C75</f>
         <v>%</v>
       </c>
-      <c r="E8" t="str">
-        <f>'M6'!D75</f>
-        <v>Weight binder</v>
-      </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="31"/>
-      <c r="Q8">
-        <v>15</v>
-      </c>
-      <c r="R8">
-        <v>15</v>
-      </c>
-      <c r="S8">
-        <v>2</v>
-      </c>
-      <c r="T8">
-        <f>SUM(Q8*R8*S8)</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="36"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="31"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="17">
+      <c r="G8" s="75" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="63"/>
+    </row>
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="34"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="37"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="26"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="54">
         <v>8</v>
       </c>
       <c r="D10" t="str">
         <f>'M6'!C77</f>
         <v>%</v>
       </c>
-      <c r="E10" t="str">
-        <f>'M6'!D77</f>
-        <v>Weight binder</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="31"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C11" s="36"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="31"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="31"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" t="str">
+      <c r="G10" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="32"/>
+      <c r="N10" s="69">
+        <v>1</v>
+      </c>
+      <c r="O10" s="33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="34"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="49"/>
+      <c r="G11" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="66">
+        <f>J10*E33</f>
+        <v>0.22853545611320927</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" s="26"/>
+      <c r="N11" s="66">
+        <f>N10*E33</f>
+        <v>2.2853545611320927</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="52"/>
+      <c r="G12" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="67">
+        <f>J10*$D$34</f>
+        <v>2.4530000000000003</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="67">
+        <f>N10*$D$34</f>
+        <v>24.53</v>
+      </c>
+      <c r="O12" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="34" t="str">
         <f>'M6'!A78</f>
         <v>Water</v>
       </c>
-      <c r="C13" s="17">
+      <c r="B13" s="26"/>
+      <c r="C13" s="35">
         <v>0.4</v>
       </c>
       <c r="D13" t="str">
         <f>'M6'!C78</f>
         <v>-</v>
       </c>
-      <c r="E13" t="str">
-        <f>'M6'!D78</f>
-        <v>wb</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="31"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="G13" s="34"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="41"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="17">
+      <c r="B14" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="35">
         <v>0.88500000000000001</v>
       </c>
       <c r="D14" t="str">
         <f>'M6'!C79</f>
         <v>%</v>
       </c>
-      <c r="E14" t="str">
-        <f>'M6'!D79</f>
-        <v>weight_solution_adm/weight_dry_binder</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="N14" s="31"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="G14" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="68">
+        <v>0.25</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="26"/>
+      <c r="N14" s="68">
+        <v>2</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="26">
+      <c r="B15" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="55">
         <f>0.105/0.3</f>
         <v>0.35</v>
       </c>
@@ -3878,367 +4211,400 @@
         <f>'M6'!C80</f>
         <v>%</v>
       </c>
-      <c r="E15" t="str">
-        <f>'M6'!D80</f>
-        <v>weight_solution_adm/weight_dry_binder</v>
-      </c>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C16" s="38"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="G15" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="66">
+        <f>J14*E33</f>
+        <v>0.57133864028302317</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M15" s="26"/>
+      <c r="N15" s="66">
+        <f>N14*E33</f>
+        <v>4.5707091222641854</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="34"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="50"/>
+      <c r="G16" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="67">
+        <f>J14*$D$34</f>
+        <v>6.1325000000000003</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="M16" s="26"/>
+      <c r="N16" s="67">
+        <f>N14*$D$34</f>
+        <v>49.06</v>
+      </c>
+      <c r="O16" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="52"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="65"/>
+      <c r="O17" s="71"/>
+    </row>
+    <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="17">
+      <c r="B18" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="40">
         <v>4</v>
       </c>
       <c r="D18" t="str">
         <f>'M6'!C82</f>
         <v>%</v>
       </c>
-      <c r="E18" t="str">
-        <f>'M6'!D82</f>
-        <v>weight_solution_adm/weight_dry_binder</v>
-      </c>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="str">
+      <c r="G18" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18" s="26"/>
+      <c r="N18" s="68">
+        <v>3</v>
+      </c>
+      <c r="O18" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G19" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="66">
+        <f>J18*E33</f>
+        <v>1.1426772805660463</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="M19" s="26"/>
+      <c r="N19" s="66">
+        <f>N18*E33</f>
+        <v>6.856063683396278</v>
+      </c>
+      <c r="O19" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="76" t="str">
         <f>'M6'!A84</f>
         <v>Recipe</v>
       </c>
-      <c r="C20" t="str">
+      <c r="B20" s="77"/>
+      <c r="C20" s="78" t="str">
         <f>'M6'!B84</f>
         <v>Mass [g]</v>
       </c>
-      <c r="D20">
-        <f>'M6'!C84</f>
-        <v>10</v>
-      </c>
-      <c r="E20" t="str">
-        <f>'M6'!D84</f>
-        <v>L</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="J20" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="K20" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="L20" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="M20" s="33"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="F21" s="29"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="F20" s="60"/>
+      <c r="G20" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="72">
+        <f>J18*$D$34</f>
+        <v>12.265000000000001</v>
+      </c>
+      <c r="K20" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="39"/>
+      <c r="N20" s="72">
+        <f>N18*$D$34</f>
+        <v>73.59</v>
+      </c>
+      <c r="O20" s="73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="56"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="64"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="44">
         <f>'M6'!B85</f>
         <v>13676</v>
       </c>
-      <c r="F22" s="30">
-        <f>'M6'!L43</f>
-        <v>1367.6</v>
-      </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33">
-        <v>1</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L22" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M22" s="33"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="61"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="27">
+      <c r="B23" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="44">
         <f>'M6'!B86</f>
         <v>5923.0532074003595</v>
       </c>
-      <c r="F23" s="30">
-        <f>'M6'!L44</f>
-        <v>592.305320740036</v>
-      </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33">
-        <f>SUM(J22+1)</f>
-        <v>2</v>
-      </c>
-      <c r="K23" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L23" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="27"/>
-      <c r="F24" s="30">
-        <f>'M6'!L45</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33">
-        <f t="shared" ref="J24:J37" si="0">SUM(J23+1)</f>
-        <v>3</v>
-      </c>
-      <c r="K24" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L24" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M24" s="33"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="27">
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="61"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+    </row>
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="34"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="44"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="57">
         <f>'M6'!B88</f>
         <v>515.04810499133555</v>
       </c>
-      <c r="F25" s="30">
-        <f>'M6'!L46</f>
-        <v>51.504810499133555</v>
-      </c>
-      <c r="H25" s="31"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L25" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="27"/>
-      <c r="F26" s="30"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="33"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="61"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="58"/>
+      <c r="F26" s="61"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="27"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="27">
+      <c r="B27" s="26"/>
+      <c r="C27" s="44">
         <f>'M6'!B89</f>
         <v>2402.4096952255231</v>
       </c>
-      <c r="F27" s="30">
-        <f>'M6'!L47</f>
-        <v>257.52405249566777</v>
-      </c>
-      <c r="H27" s="31"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33">
-        <f>SUM(J25+1)</f>
-        <v>5</v>
-      </c>
-      <c r="K27" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L27" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M27" s="33"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="61"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="27"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="23">
+      <c r="B28" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="45">
         <f>'M6'!B90</f>
         <v>56.977196614666504</v>
       </c>
-      <c r="F28" s="30">
-        <f>'M6'!L48</f>
-        <v>1.7093158984399948</v>
-      </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K28" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L28" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M28" s="33"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" t="str">
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="61"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="27"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="53" t="str">
         <f>'M6'!A91</f>
         <v>Sucrose</v>
       </c>
-      <c r="B29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="23">
+      <c r="B29" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="59">
         <f>'M6'!B91</f>
         <v>22.533354593370927</v>
       </c>
-      <c r="F29" s="30">
-        <f>'M6'!L49</f>
-        <v>0.67600063780112774</v>
-      </c>
-      <c r="H29" s="31"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="K29" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L29" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M29" s="33"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="F30" s="30">
-        <f>'M6'!L50</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="31"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K30" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L30" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M30" s="33"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="61"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="27"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="45"/>
+      <c r="F30" s="61"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B31" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="23">
+      <c r="B31" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="46">
         <f>'M6'!B93</f>
         <v>257.52405249566777</v>
       </c>
-      <c r="F31" s="30">
-        <f>'M6'!L51</f>
-        <v>14.035060861013894</v>
-      </c>
-      <c r="H31" s="31"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K31" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L31" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M31" s="33"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="61"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="27"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="F32" s="1"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="K32" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L32" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M32" s="33"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="27"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -4258,52 +4624,38 @@
       <c r="F33" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="31"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="K33" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L33" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M33" s="33"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="27"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34">
         <v>24.53</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H34" s="31"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="33"/>
+        <v>113</v>
+      </c>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="27"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H35" s="31"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33">
-        <f>SUM(J33+1)</f>
-        <v>12</v>
-      </c>
-      <c r="K35" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L35" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M35" s="33"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="27"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -4316,19 +4668,12 @@
       <c r="E36" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="K36" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L36" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M36" s="33"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="27"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -4341,334 +4686,77 @@
       <c r="E37" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="31"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="K37" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L37" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="M37" s="33"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="27"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H38" s="31"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="I39" t="s">
-        <v>80</v>
-      </c>
-      <c r="J39" s="33"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="28">
-        <f>D39*E33</f>
-        <v>0.22853545611320927</v>
-      </c>
-      <c r="E40" t="s">
-        <v>106</v>
-      </c>
-      <c r="F40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H40" s="28">
-        <f>H39*E33</f>
-        <v>1.1426772805660463</v>
-      </c>
-      <c r="I40" t="s">
-        <v>106</v>
-      </c>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="23">
-        <f>D39*$D$34</f>
-        <v>2.4530000000000003</v>
-      </c>
-      <c r="E41" t="s">
-        <v>79</v>
-      </c>
-      <c r="F41" t="s">
-        <v>112</v>
-      </c>
-      <c r="H41" s="23">
-        <f>H39*$D$34</f>
-        <v>12.265000000000001</v>
-      </c>
-      <c r="I41" t="s">
-        <v>79</v>
-      </c>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H42" s="31"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="E43" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H43" s="26">
-        <v>0.6</v>
-      </c>
-      <c r="I43" t="s">
-        <v>80</v>
-      </c>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" s="28">
-        <f>D43*E33</f>
-        <v>0.45707091222641855</v>
-      </c>
-      <c r="E44" t="s">
-        <v>106</v>
-      </c>
-      <c r="F44" t="s">
-        <v>105</v>
-      </c>
-      <c r="H44" s="28">
-        <f>H43*E33</f>
-        <v>1.3712127366792555</v>
-      </c>
-      <c r="I44" t="s">
-        <v>106</v>
-      </c>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="23">
-        <f>D43*$D$34</f>
-        <v>4.9060000000000006</v>
-      </c>
-      <c r="E45" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" t="s">
-        <v>112</v>
-      </c>
-      <c r="H45" s="23">
-        <f>H43*$D$34</f>
-        <v>14.718</v>
-      </c>
-      <c r="I45" t="s">
-        <v>79</v>
-      </c>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="31"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="26"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="E47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" t="s">
-        <v>104</v>
-      </c>
-      <c r="H47" s="26">
-        <v>0.8</v>
-      </c>
-      <c r="I47" t="s">
-        <v>80</v>
-      </c>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="28">
-        <f>D47*E33</f>
-        <v>0.68560636833962774</v>
-      </c>
-      <c r="E48" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" t="s">
-        <v>105</v>
-      </c>
-      <c r="H48" s="28">
-        <f>H47*E33</f>
-        <v>1.8282836489056742</v>
-      </c>
-      <c r="I48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="23">
-        <f>D47*$D$34</f>
-        <v>7.359</v>
-      </c>
-      <c r="E49" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" t="s">
-        <v>112</v>
-      </c>
-      <c r="H49" s="23">
-        <f>H47*$D$34</f>
-        <v>19.624000000000002</v>
-      </c>
-      <c r="I49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H50" s="31"/>
-      <c r="I50" s="33"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>104</v>
-      </c>
-      <c r="D51" s="26">
-        <v>0.4</v>
-      </c>
-      <c r="E51" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" t="s">
-        <v>104</v>
-      </c>
-      <c r="H51" s="26">
-        <v>1</v>
-      </c>
-      <c r="I51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="28">
-        <f>D51*E33</f>
-        <v>0.91414182445283709</v>
-      </c>
-      <c r="E52" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" t="s">
-        <v>105</v>
-      </c>
-      <c r="H52" s="28">
-        <f>H51*E33</f>
-        <v>2.2853545611320927</v>
-      </c>
-      <c r="I52" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" s="23">
-        <f>D51*$D$34</f>
-        <v>9.8120000000000012</v>
-      </c>
-      <c r="E53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F53" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="23">
-        <f>H51*$D$34</f>
-        <v>24.53</v>
-      </c>
-      <c r="I53" t="s">
-        <v>79</v>
-      </c>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>

</xml_diff>